<commit_message>
oneamp lig adaptor received
</commit_message>
<xml_diff>
--- a/oneamp/oneamp_bar_lig_adaptor_24.xlsx
+++ b/oneamp/oneamp_bar_lig_adaptor_24.xlsx
@@ -1,15 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taol9/gitsss/yo/oneamp/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03ECE9CE-0BAD-2E46-9DA6-2E1A02E3E288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="2000" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -241,8 +257,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,6 +321,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -351,7 +375,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -383,9 +407,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -417,6 +459,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -592,14 +652,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -607,7 +674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -618,7 +685,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -629,7 +696,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -640,7 +707,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -651,7 +718,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -662,7 +729,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -673,7 +740,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -684,7 +751,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -695,7 +762,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -706,7 +773,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -717,7 +784,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -728,7 +795,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -739,7 +806,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -750,7 +817,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -761,7 +828,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -772,7 +839,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -783,7 +850,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -794,7 +861,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -805,7 +872,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
@@ -816,7 +883,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
@@ -827,7 +894,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -838,7 +905,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -849,7 +916,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
@@ -860,7 +927,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>